<commit_message>
fix: key change for leps/plants to include hyphen
</commit_message>
<xml_diff>
--- a/src/main/resources/finalPlantList.xlsx
+++ b/src/main/resources/finalPlantList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharjianto/Documents/S21/275labs/project-team-11-1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AF37B6-C330-144D-921F-8450C6EF69D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCD4ECD-7430-724F-A836-5E6219B89FD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="500" windowWidth="14280" windowHeight="16060" xr2:uid="{CC028ED6-6576-7E41-9C79-63CA21B893D4}"/>
+    <workbookView xWindow="10420" yWindow="500" windowWidth="14280" windowHeight="16060" xr2:uid="{CC028ED6-6576-7E41-9C79-63CA21B893D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="213">
   <si>
     <t>Asteraceae</t>
   </si>
@@ -585,9 +585,6 @@
     <t>Native Delaware Leps</t>
   </si>
   <si>
-    <t>Image</t>
-  </si>
-  <si>
     <t>Amaranthaceae </t>
   </si>
   <si>
@@ -670,6 +667,12 @@
   </si>
   <si>
     <t>stellata</t>
+  </si>
+  <si>
+    <t>Cropped Image</t>
+  </si>
+  <si>
+    <t>Full Image</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFE0C99-2D93-6B49-A62F-76E979F00191}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="F2" sqref="F2:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,9 +1117,11 @@
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>153</v>
       </c>
@@ -1133,10 +1138,13 @@
         <v>182</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1170,9 +1178,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>51</v>
@@ -1187,9 +1195,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>51</v>
@@ -1204,7 +1212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1229,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -1255,7 +1263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -1289,7 +1297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>48</v>
       </c>
@@ -1306,7 +1314,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1323,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1357,7 +1365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1374,7 +1382,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>168</v>
       </c>
@@ -1393,13 +1401,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>1</v>
@@ -1410,7 +1418,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>60</v>
@@ -1461,7 +1469,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>108</v>
@@ -1529,7 +1537,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>99</v>
@@ -1563,10 +1571,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>201</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>173</v>
@@ -1604,7 +1612,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>5</v>
@@ -1621,7 +1629,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>5</v>
@@ -1700,13 +1708,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>1</v>
@@ -1989,7 +1997,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>34</v>
@@ -2006,7 +2014,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>34</v>
@@ -2057,7 +2065,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>145</v>
@@ -2074,7 +2082,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>61</v>
@@ -2176,13 +2184,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>5</v>
@@ -2193,7 +2201,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>80</v>
@@ -2210,7 +2218,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>80</v>
@@ -2278,13 +2286,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B69" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C69" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>1</v>
@@ -2295,13 +2303,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B70" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>1</v>
@@ -2329,7 +2337,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>56</v>
@@ -2369,7 +2377,7 @@
         <v>29</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>1</v>
@@ -2386,7 +2394,7 @@
         <v>29</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>1</v>
@@ -2403,7 +2411,7 @@
         <v>29</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>1</v>
@@ -2420,7 +2428,7 @@
         <v>29</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>1</v>
@@ -2539,7 +2547,7 @@
         <v>63</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>1</v>
@@ -2556,7 +2564,7 @@
         <v>63</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>1</v>
@@ -2618,7 +2626,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>64</v>
@@ -2669,7 +2677,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>133</v>
@@ -2686,7 +2694,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>133</v>
@@ -2703,7 +2711,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>133</v>

</xml_diff>